<commit_message>
more flexible grouping - with safeguards agains empty vector
</commit_message>
<xml_diff>
--- a/inst/extdata/newresconst.xlsx
+++ b/inst/extdata/newresconst.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Data\r-projects\unpivotr-dev\unpivotr\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30DB6E17-A273-4514-9D6D-480D38AADCB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A86A2A1-3BD8-4982-947E-E4E2C7A3BAB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 - Permits" sheetId="1" r:id="rId1"/>
@@ -26,14 +26,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Table 5 - Completions'!$A$1:$M$75</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -622,13 +614,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="171" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="0.0%"/>
-    <numFmt numFmtId="174" formatCode="\±\ #,##0.0\ ;\-#,##0.0\ ;0.0\ ;@\ "/>
-    <numFmt numFmtId="175" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="\±\ #,##0.0\ ;\-#,##0.0\ ;0.0\ ;@\ "/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -969,7 +961,7 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -991,112 +983,112 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="9" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="13" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="14" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="14" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="7" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="7" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="13" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="9" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="13" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="13" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="12" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="19" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="21" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="22" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="21" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="8" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="23" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="23" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="23" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="23" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="23" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="23" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="23" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="23" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="12" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="19" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="19" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="21" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="21" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="23" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="23" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="21" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1105,14 +1097,14 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="172" fontId="21" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="21" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="22" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="22" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="174" fontId="21" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="21" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="21" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="21" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1471,11 +1463,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3653,11 +3645,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="B33:E33"/>
@@ -3665,6 +3652,11 @@
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="J33:K33"/>
     <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="A8:A22">
     <cfRule type="cellIs" dxfId="9" priority="4" operator="between">
@@ -3679,7 +3671,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A76" r:id="rId1"/>
+    <hyperlink ref="A76" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0" header="0.3" footer="0.3"/>
@@ -3688,7 +3680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N77"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -5883,11 +5875,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="A73:M73"/>
     <mergeCell ref="A33:A34"/>
@@ -5896,6 +5883,11 @@
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="J33:K33"/>
     <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="A8:A22">
     <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
@@ -5910,7 +5902,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A77" r:id="rId1"/>
+    <hyperlink ref="A77" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0" header="0.3" footer="0.3"/>
@@ -5919,7 +5911,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N75"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -8097,11 +8089,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="B33:E33"/>
@@ -8109,6 +8096,11 @@
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="J33:K33"/>
     <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="A8:A22">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="between">
@@ -8123,7 +8115,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A75" r:id="rId1"/>
+    <hyperlink ref="A75" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0" header="0.3" footer="0.3"/>
@@ -8132,7 +8124,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N75"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10305,11 +10297,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="B33:E33"/>
@@ -10317,6 +10304,11 @@
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="J33:K33"/>
     <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="A8:A22">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="between">
@@ -10331,7 +10323,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A75" r:id="rId1"/>
+    <hyperlink ref="A75" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0" header="0.3" footer="0.3"/>
@@ -10340,7 +10332,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N75"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -12518,11 +12510,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="B33:E33"/>
@@ -12530,6 +12517,11 @@
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="J33:K33"/>
     <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="A8:A22">
     <cfRule type="cellIs" dxfId="1" priority="4" operator="between">
@@ -12544,7 +12536,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A75" r:id="rId1"/>
+    <hyperlink ref="A75" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0" header="0.3" footer="0.3"/>

</xml_diff>